<commit_message>
Done Enunciado del Proyecto
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{67271C5B-1657-4DE8-B140-42E3575B437A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D0933440-806F-4449-BECB-F650D451752F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Fase 5</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -373,38 +376,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -462,196 +448,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -988,7 +784,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,138 +794,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1137,27 +935,27 @@
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C18">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1186,7 +984,7 @@
       <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1195,7 +993,7 @@
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1204,7 +1002,7 @@
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1213,7 +1011,7 @@
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1222,7 +1020,7 @@
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1231,7 +1029,7 @@
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1240,7 +1038,7 @@
       <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1249,14 +1047,14 @@
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1265,7 +1063,7 @@
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1274,7 +1072,7 @@
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1283,7 +1081,7 @@
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1292,7 +1090,7 @@
       <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1301,7 +1099,7 @@
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C14">

</xml_diff>

<commit_message>
Empezado diseños casos de pruebas unit
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D0933440-806F-4449-BECB-F650D451752F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7038DED9-F798-47AB-9E8A-A05CE6E70482}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -275,6 +275,36 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Métodos</t>
+  </si>
+  <si>
+    <t>agregarArista(deVertice, aVertice, ponderación)</t>
+  </si>
+  <si>
+    <t>agregarVertice(Vertice)</t>
+  </si>
+  <si>
+    <t>eliminarArista()</t>
+  </si>
+  <si>
+    <t>eliminarVertice()</t>
+  </si>
+  <si>
+    <t>darVertice(Ver)</t>
+  </si>
+  <si>
+    <t>Algotirmo BFS</t>
+  </si>
+  <si>
+    <t>Algoritmo DFS</t>
+  </si>
+  <si>
+    <t>Algoritmo Dijsktra</t>
+  </si>
+  <si>
+    <t>Algoritmo Prim</t>
   </si>
 </sst>
 </file>
@@ -380,11 +410,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,125 +823,157 @@
     <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="6"/>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6"/>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="6"/>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="6"/>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="6"/>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -920,14 +982,14 @@
       <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Cambio de lugar UML y update ToDo
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7038DED9-F798-47AB-9E8A-A05CE6E70482}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EC47DA4-7FCD-4DB7-9A86-08BA5EAD4C9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>Algoritmo Prim</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>Camila</t>
   </si>
 </sst>
 </file>
@@ -814,7 +820,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +844,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" t="s">
         <v>51</v>
       </c>
@@ -915,6 +926,9 @@
       <c r="C9" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
       <c r="F9" t="s">
         <v>58</v>
       </c>
@@ -926,6 +940,9 @@
       </c>
       <c r="C10" s="6" t="s">
         <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Terminados diseños operaciones estructurales
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EC47DA4-7FCD-4DB7-9A86-08BA5EAD4C9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{281B98B6-F863-4C72-9614-0EB54132DFA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -820,7 +820,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +881,9 @@
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F5" t="s">
         <v>54</v>
       </c>
@@ -891,7 +893,9 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F6" t="s">
         <v>55</v>
       </c>
@@ -901,7 +905,9 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="F7" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Exportado pdf Primera Entrega
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{281B98B6-F863-4C72-9614-0EB54132DFA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A6720A2-CFCF-4F08-BAE4-CC3F761ACB8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -277,40 +277,13 @@
     <t>x</t>
   </si>
   <si>
-    <t>Métodos</t>
-  </si>
-  <si>
-    <t>agregarArista(deVertice, aVertice, ponderación)</t>
-  </si>
-  <si>
-    <t>agregarVertice(Vertice)</t>
-  </si>
-  <si>
-    <t>eliminarArista()</t>
-  </si>
-  <si>
-    <t>eliminarVertice()</t>
-  </si>
-  <si>
-    <t>darVertice(Ver)</t>
-  </si>
-  <si>
-    <t>Algotirmo BFS</t>
-  </si>
-  <si>
-    <t>Algoritmo DFS</t>
-  </si>
-  <si>
-    <t>Algoritmo Dijsktra</t>
-  </si>
-  <si>
-    <t>Algoritmo Prim</t>
-  </si>
-  <si>
     <t>Javier</t>
   </si>
   <si>
     <t>Camila</t>
+  </si>
+  <si>
+    <t>Palma</t>
   </si>
 </sst>
 </file>
@@ -817,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,17 +802,14 @@
     <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
-      <c r="F1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -848,33 +818,30 @@
         <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="6"/>
-      <c r="F3" t="s">
+      <c r="D3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="6"/>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -884,11 +851,11 @@
       <c r="C5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -896,11 +863,11 @@
       <c r="C6" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -908,21 +875,23 @@
       <c r="C7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="F8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -933,13 +902,10 @@
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -948,20 +914,17 @@
         <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -970,28 +933,28 @@
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Creado proyecto en Maven
Y tambien el ToDo el método de la ingeniería
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A6720A2-CFCF-4F08-BAE4-CC3F761ACB8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3A87EC52-FDB8-4075-9AE7-7F191B6C6E9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" firstSheet="1" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
     <sheet name="Rúbrica" sheetId="2" r:id="rId2"/>
+    <sheet name="Método" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -284,6 +285,51 @@
   </si>
   <si>
     <t>Palma</t>
+  </si>
+  <si>
+    <t>Definición del problema</t>
+  </si>
+  <si>
+    <t>Justificación</t>
+  </si>
+  <si>
+    <t>Requerimientos funcionales</t>
+  </si>
+  <si>
+    <t>Contexto</t>
+  </si>
+  <si>
+    <t>Teoría</t>
+  </si>
+  <si>
+    <t>BFS Y DFS</t>
+  </si>
+  <si>
+    <t>Camino min</t>
+  </si>
+  <si>
+    <t>Árboles de recubrimiento</t>
+  </si>
+  <si>
+    <t>Al menos 7 alternativas</t>
+  </si>
+  <si>
+    <t>Método de generación de ideas</t>
+  </si>
+  <si>
+    <t>Al menos 7 ideas</t>
+  </si>
+  <si>
+    <t>Descarte de ideas</t>
+  </si>
+  <si>
+    <t>Diseño preliminar otras ideas</t>
+  </si>
+  <si>
+    <t>Criterios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asignar valores </t>
   </si>
 </sst>
 </file>
@@ -790,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,14 +848,14 @@
     <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -821,27 +867,37 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -855,7 +911,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -867,7 +923,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -879,7 +935,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -891,7 +947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -905,7 +961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -917,14 +973,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -933,28 +989,28 @@
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>48</v>
@@ -1015,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F0590B-C829-4258-AAC3-B4B32338B06B}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,4 +1214,122 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Informe y ToDo
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{688F4B3F-E892-41EF-89AD-3A26587A75F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2BF311E9-9522-437D-8D8B-1CB087A96FC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -432,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -444,20 +444,43 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -485,16 +508,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -910,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,18 +934,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D2" t="s">
@@ -944,7 +957,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D3" t="s">
@@ -959,7 +972,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
@@ -976,7 +989,7 @@
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D5" t="s">
@@ -988,7 +1001,7 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D6" t="s">
@@ -1000,7 +1013,7 @@
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
@@ -1012,7 +1025,7 @@
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D8" t="s">
@@ -1026,7 +1039,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D9" t="s">
@@ -1038,7 +1051,7 @@
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D10" t="s">
@@ -1046,11 +1059,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1059,35 +1072,37 @@
       <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -1096,28 +1111,28 @@
       <c r="B17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1125,49 +1140,49 @@
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C17 C20">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1180,13 +1195,14 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" customWidth="1"/>
     <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1196,7 +1212,9 @@
       <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1205,7 +1223,9 @@
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1214,7 +1234,7 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1223,7 +1243,9 @@
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1232,7 +1254,7 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1241,7 +1263,7 @@
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1250,7 +1272,7 @@
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1259,14 +1281,14 @@
       <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1275,7 +1297,7 @@
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1284,7 +1306,7 @@
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1293,7 +1315,7 @@
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1302,7 +1324,7 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1311,11 +1333,11 @@
       <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1326,39 +1348,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1366,7 +1401,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1374,42 +1409,51 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -1445,6 +1489,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fase 2 método terminada y comenzada fase 3
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2BF311E9-9522-437D-8D8B-1CB087A96FC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{49128EE8-936A-4FC3-B99C-97C576FCFDBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Árboles de recubrimiento</t>
   </si>
   <si>
-    <t>Al menos 7 alternativas</t>
-  </si>
-  <si>
     <t>Método de generación de ideas</t>
   </si>
   <si>
@@ -342,6 +339,15 @@
   </si>
   <si>
     <t>Pruebas unitarias MA</t>
+  </si>
+  <si>
+    <t>Revisar en el postmortem</t>
+  </si>
+  <si>
+    <t>Para la guía</t>
+  </si>
+  <si>
+    <t>Para los tesoros</t>
   </si>
 </sst>
 </file>
@@ -447,13 +453,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -923,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,11 +940,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1059,11 +1065,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1109,28 +1115,28 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -1195,14 +1201,14 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" customWidth="1"/>
     <col min="2" max="2" width="61.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="8"/>
+    <col min="3" max="3" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1212,7 +1218,7 @@
       <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1223,7 +1229,7 @@
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1234,7 +1240,7 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1243,7 +1249,7 @@
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1254,7 +1260,7 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1263,7 +1269,7 @@
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1272,7 +1278,7 @@
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1281,14 +1287,14 @@
       <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="7"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1297,7 +1303,9 @@
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1306,7 +1314,7 @@
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1315,7 +1323,7 @@
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1324,7 +1332,7 @@
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1333,7 +1341,7 @@
       <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C14">
@@ -1348,114 +1356,126 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="7"/>
+    <col min="3" max="3" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>62</v>
+      <c r="B16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -1465,12 +1485,12 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -1480,12 +1500,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminado zip Entrega 2
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{49128EE8-936A-4FC3-B99C-97C576FCFDBE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{929C4DC2-E028-4C39-96F0-E5D9F10D3EC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -354,7 +354,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +380,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -438,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,6 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1096,9 @@
       <c r="B13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -1201,7 +1212,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1325,9 @@
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1356,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1383,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -1404,17 +1417,28 @@
         <v>48</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>48</v>
@@ -1422,12 +1446,15 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>48</v>
@@ -1435,7 +1462,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>48</v>
@@ -1443,69 +1470,82 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>59</v>
+      <c r="A12" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>48</v>
+      <c r="A15" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
         <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1515,5 +1555,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update diseños de casos pruebas
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{929C4DC2-E028-4C39-96F0-E5D9F10D3EC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7076E4BC-8912-4E63-8B78-2648AE31EB74}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t>Para los tesoros</t>
+  </si>
+  <si>
+    <t>Actualizar el TAD</t>
+  </si>
+  <si>
+    <t>Actualizar el diagrama</t>
+  </si>
+  <si>
+    <t>Interfaz completa</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -467,15 +476,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -936,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,11 +1049,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1074,11 +1174,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1150,6 +1250,27 @@
         <v>70</v>
       </c>
       <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1157,49 +1278,82 @@
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C17 C20">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>$I$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>$I$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>$I$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1358,7 +1512,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1371,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1537,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -1418,7 +1572,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1477,7 +1631,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1501,7 +1655,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1525,7 +1679,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1550,7 +1704,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Terminados diesños algoritmos de recubrimiento min :+1:
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A26F2CA-3750-4AD3-A515-0CFF2AB5F23D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00E2E744-7791-4649-8CF9-6D53802603A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1222,9 @@
       <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D16" t="s">
         <v>77</v>
       </c>
@@ -1234,14 +1236,18 @@
       <c r="B17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -1372,7 +1378,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Método e interfaz
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00E2E744-7791-4649-8CF9-6D53802603A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3A61D2EA-8F4B-4296-B88C-3BB22C6B88A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1378,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added eliminar y añadir pasillo y habitación
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AAC34936-6E67-4566-A492-35F62538E9C9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D3D62119-04EC-431E-AB59-443847CE49DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="3" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
     <sheet name="Rúbrica" sheetId="2" r:id="rId2"/>
     <sheet name="Método" sheetId="3" r:id="rId3"/>
+    <sheet name="Conexion a interfaz" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -360,6 +361,33 @@
   </si>
   <si>
     <t>REVISAR LAS PRUEBAS, ACOMODAR NOMBRES</t>
+  </si>
+  <si>
+    <t>Camino mas corto de min desde una habitacion hasta la salida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camino mas corto entre dos habitaciones </t>
+  </si>
+  <si>
+    <t>Transmitir mensaje de cierre</t>
+  </si>
+  <si>
+    <t>Añadir una habitacion</t>
+  </si>
+  <si>
+    <t>Eliminar habitacion</t>
+  </si>
+  <si>
+    <t>Registrar tesoros encontrados</t>
+  </si>
+  <si>
+    <t>Visualizar los tesoros</t>
+  </si>
+  <si>
+    <t>Añadir pasillo</t>
+  </si>
+  <si>
+    <t>Eliminar Pasillo</t>
   </si>
 </sst>
 </file>
@@ -488,7 +516,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1041,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,82 +1330,82 @@
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C17 C20">
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1379,7 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F0590B-C829-4258-AAC3-B4B32338B06B}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1568,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1722,11 +1760,95 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAEB2D8-29A9-48D5-83D6-66D2F2DEA5E6}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added documentación para IGraph
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D3D62119-04EC-431E-AB59-443847CE49DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E4ED652B-2E27-43A5-990C-69CFC01408FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="3" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F0590B-C829-4258-AAC3-B4B32338B06B}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAEB2D8-29A9-48D5-83D6-66D2F2DEA5E6}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,10 +1795,16 @@
       <c r="A2" t="s">
         <v>79</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Empezados diseños casos MansionTest
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\AEDFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C280F0-AFCC-4357-BEB8-1241C836DACA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7608B15D-C7D0-4018-858E-CE33CBF9B0A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="2" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="3" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Soluciona el problema planteado completamente</t>
   </si>
   <si>
-    <t>Elementos adicionales del método de la ingeniería</t>
-  </si>
-  <si>
     <t>Fase 2. Recopilación de la información necesaria</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
     <t>REVISAR LAS PRUEBAS, ACOMODAR NOMBRES</t>
   </si>
   <si>
-    <t>Camino mas corto de min desde una habitacion hasta la salida</t>
-  </si>
-  <si>
     <t xml:space="preserve">Camino mas corto entre dos habitaciones </t>
   </si>
   <si>
@@ -388,6 +382,18 @@
   </si>
   <si>
     <t>Eliminar Pasillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementacion </t>
+  </si>
+  <si>
+    <t>Diseño test</t>
+  </si>
+  <si>
+    <t>Test implementado</t>
+  </si>
+  <si>
+    <t>Camino mas corto en min desde una habitacion hasta la salida</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -512,11 +518,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1079,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,10 +1131,10 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,13 +1143,13 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,13 +1158,13 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,10 +1175,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1158,10 +1187,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1170,10 +1199,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,10 +1211,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,10 +1225,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,10 +1237,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,43 +1255,43 @@
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1270,57 +1299,57 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -1330,82 +1359,82 @@
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C17 C20">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1415,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F0590B-C829-4258-AAC3-B4B32338B06B}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1465,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1476,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1467,7 +1496,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1478,7 +1507,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1488,7 +1517,9 @@
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1498,7 +1529,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1508,67 +1539,64 @@
       <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="C1:C13">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1581,7 +1609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1594,64 +1622,64 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,108 +1687,108 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1771,92 +1799,133 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAEB2D8-29A9-48D5-83D6-66D2F2DEA5E6}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="7"/>
+    <col min="2" max="2" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="B10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:D10">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Terminados diseños de casos de pruebas para TestMansion
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7608B15D-C7D0-4018-858E-CE33CBF9B0A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E79CB44-E197-4182-BFB3-9B7A35ECAC82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="3" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="89">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -515,27 +515,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1119,11 +1109,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1244,11 +1234,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1359,82 +1349,82 @@
     <mergeCell ref="A11:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C17 C20">
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>$I$1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1596,7 +1586,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C13">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1788,7 +1778,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1802,7 +1792,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1805,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -1829,99 +1819,113 @@
       <c r="A2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="B3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="11"/>
+      <c r="B5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="11"/>
+      <c r="B6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="B8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added prueba 4/8 testMansion
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0993DA0F-A50D-4030-A389-0A7D9C0FA7B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EBD7F9F7-33D4-4F8E-8463-ED69EB88A833}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="3" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Entregables" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="92">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -1107,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAEB2D8-29A9-48D5-83D6-66D2F2DEA5E6}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1883,9 @@
       <c r="C5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1895,7 +1897,9 @@
       <c r="C6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1931,7 +1935,9 @@
       <c r="C9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1943,7 +1949,9 @@
       <c r="C10" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
Update método de la ingenieria
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\AED\LABS\AEDFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2A189634-EC62-4240-A43F-02FEBC82A390}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B8815D11-D518-4794-9969-BDB43FD8CBAA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" activeTab="3" xr2:uid="{5E521AF5-00F6-43AE-BC10-647F1631B4CF}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>Primera entrega</t>
   </si>
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>Pruebas unitarias MA</t>
-  </si>
-  <si>
-    <t>Revisar en el postmortem</t>
   </si>
   <si>
     <t>Para la guía</t>
@@ -1107,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B79DB2-2487-45AA-95D9-C4A21D06912C}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1201,7 @@
         <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1219,7 +1216,7 @@
         <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1236,7 +1233,7 @@
         <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1251,7 +1248,7 @@
         <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,21 +1283,27 @@
       <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -1343,7 +1346,7 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>47</v>
@@ -1352,14 +1355,16 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>47</v>
@@ -1459,7 +1464,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1503,9 @@
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1584,7 +1591,9 @@
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1593,7 +1602,9 @@
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1619,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A06401-ED22-4000-82AB-F8B94124640C}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1643,7 @@
     <col min="3" max="3" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>42</v>
       </c>
@@ -1640,7 +1651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1648,18 +1659,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1667,7 +1675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>43</v>
       </c>
@@ -1675,7 +1683,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1694,7 +1702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1702,7 +1710,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1710,7 +1718,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1718,7 +1726,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1726,41 +1734,50 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>47</v>
@@ -1771,20 +1788,26 @@
         <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>46</v>
       </c>
+      <c r="C18" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>47</v>
@@ -1795,7 +1818,10 @@
         <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1840,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,18 +1854,18 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>47</v>
@@ -1853,7 +1879,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>47</v>
@@ -1867,7 +1893,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>47</v>
@@ -1879,7 +1905,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>47</v>
@@ -1893,7 +1919,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>47</v>
@@ -1907,7 +1933,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>47</v>
@@ -1919,7 +1945,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>47</v>
@@ -1931,7 +1957,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>47</v>
@@ -1945,7 +1971,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>47</v>

</xml_diff>